<commit_message>
Represent 111 rules for new gas as change in new capacity factor instead of ban
</commit_message>
<xml_diff>
--- a/InputData/elec/BBNPPTY/BAU Ban New Power Plants This Year.xlsx
+++ b/InputData/elec/BBNPPTY/BAU Ban New Power Plants This Year.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\elec\BBNPPTY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66582C1F-0C47-42E5-9226-B6D9CE2514BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3502B28A-161E-4459-AD22-FA23663F12B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Source:</t>
   </si>
@@ -132,9 +132,6 @@
   </si>
   <si>
     <t>This is a Boolean value that should be set to 0 or 1 in each year.</t>
-  </si>
-  <si>
-    <t>2028 and new combined cycle gas without CCS is banned starting in 2032.</t>
   </si>
   <si>
     <t>In the U.S., we use this to represent EPA 111 Rules. New coal without CCS is banned starting in</t>
@@ -523,7 +520,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -576,12 +573,12 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>33</v>
+      <c r="A13">
+        <v>2028</v>
       </c>
     </row>
   </sheetData>
@@ -597,8 +594,8 @@
   </sheetPr>
   <dimension ref="A1:AE25"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14:AE14"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4:AE4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -930,61 +927,61 @@
         <v>0</v>
       </c>
       <c r="M4" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N4" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O4" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P4" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q4" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R4" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S4" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T4" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U4" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V4" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W4" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X4" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y4" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z4" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA4" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB4" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC4" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD4" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE4" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Allow policy mandated capacity additions to overwrite new power plant ban, and set ban to apply to all plants from 2021-2023 (when we've already specified historical additions in input data)
</commit_message>
<xml_diff>
--- a/InputData/elec/BBNPPTY/BAU Ban New Power Plants This Year.xlsx
+++ b/InputData/elec/BBNPPTY/BAU Ban New Power Plants This Year.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\elec\BBNPPTY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3502B28A-161E-4459-AD22-FA23663F12B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7697ECBD-92C9-4103-9555-181ACE6C7B7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -519,7 +519,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -594,8 +594,8 @@
   </sheetPr>
   <dimension ref="A1:AE25"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4:AE4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -704,13 +704,13 @@
         <v>11</v>
       </c>
       <c r="B2" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" s="5">
         <v>0</v>
@@ -799,13 +799,13 @@
         <v>18</v>
       </c>
       <c r="B3" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3" s="5">
         <v>0</v>
@@ -894,13 +894,13 @@
         <v>19</v>
       </c>
       <c r="B4" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" s="5">
         <v>0</v>
@@ -989,13 +989,13 @@
         <v>5</v>
       </c>
       <c r="B5" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" s="5">
         <v>0</v>
@@ -1084,13 +1084,13 @@
         <v>1</v>
       </c>
       <c r="B6" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" s="5">
         <v>0</v>
@@ -1179,13 +1179,13 @@
         <v>12</v>
       </c>
       <c r="B7" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" s="5">
         <v>0</v>
@@ -1274,13 +1274,13 @@
         <v>3</v>
       </c>
       <c r="B8" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" s="5">
         <v>0</v>
@@ -1369,13 +1369,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" s="5">
         <v>0</v>
@@ -1464,13 +1464,13 @@
         <v>2</v>
       </c>
       <c r="B10" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" s="5">
         <v>0</v>
@@ -1559,13 +1559,13 @@
         <v>7</v>
       </c>
       <c r="B11" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" s="5">
         <v>0</v>
@@ -1654,13 +1654,13 @@
         <v>8</v>
       </c>
       <c r="B12" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" s="5">
         <v>0</v>
@@ -1749,13 +1749,13 @@
         <v>9</v>
       </c>
       <c r="B13" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" s="5">
         <v>0</v>
@@ -1844,13 +1844,13 @@
         <v>10</v>
       </c>
       <c r="B14" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" s="5">
         <v>0</v>
@@ -1939,13 +1939,13 @@
         <v>13</v>
       </c>
       <c r="B15" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15" s="5">
         <v>0</v>
@@ -2034,13 +2034,13 @@
         <v>14</v>
       </c>
       <c r="B16" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C16" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16" s="5">
         <v>0</v>
@@ -2129,13 +2129,13 @@
         <v>15</v>
       </c>
       <c r="B17" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17" s="5">
         <v>0</v>
@@ -2224,13 +2224,13 @@
         <v>16</v>
       </c>
       <c r="B18" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C18" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18" s="5">
         <v>0</v>
@@ -2319,13 +2319,13 @@
         <v>20</v>
       </c>
       <c r="B19" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C19" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19" s="5">
         <v>0</v>
@@ -2414,13 +2414,13 @@
         <v>21</v>
       </c>
       <c r="B20" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C20" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20" s="5">
         <v>0</v>
@@ -2509,13 +2509,13 @@
         <v>22</v>
       </c>
       <c r="B21" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C21" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21" s="5">
         <v>0</v>
@@ -2604,13 +2604,13 @@
         <v>23</v>
       </c>
       <c r="B22" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C22" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D22" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E22" s="5">
         <v>0</v>
@@ -2699,13 +2699,13 @@
         <v>24</v>
       </c>
       <c r="B23" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C23" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D23" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23" s="5">
         <v>0</v>
@@ -2794,13 +2794,13 @@
         <v>25</v>
       </c>
       <c r="B24" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C24" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24" s="5">
         <v>0</v>
@@ -2889,13 +2889,13 @@
         <v>26</v>
       </c>
       <c r="B25" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C25" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D25" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E25" s="5">
         <v>0</v>

</xml_diff>

<commit_message>
Remove additional EPA 111 rules impacts
</commit_message>
<xml_diff>
--- a/InputData/elec/BBNPPTY/BAU Ban New Power Plants This Year.xlsx
+++ b/InputData/elec/BBNPPTY/BAU Ban New Power Plants This Year.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\elec\BBNPPTY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7697ECBD-92C9-4103-9555-181ACE6C7B7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1254EFA1-62CF-4ED5-AAD9-5F49CA4D654B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -594,8 +594,8 @@
   </sheetPr>
   <dimension ref="A1:AE25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D25"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:AE25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -725,73 +725,73 @@
         <v>0</v>
       </c>
       <c r="I2" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J2" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K2" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L2" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M2" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N2" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O2" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P2" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q2" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R2" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S2" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T2" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U2" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V2" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W2" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X2" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y2" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z2" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA2" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB2" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC2" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD2" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE2" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
@@ -1865,73 +1865,73 @@
         <v>0</v>
       </c>
       <c r="I14" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J14" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K14" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L14" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M14" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N14" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O14" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P14" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q14" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R14" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S14" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T14" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U14" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V14" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W14" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X14" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y14" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z14" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA14" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB14" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC14" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD14" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE14" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Corrects methodological issue with ban on CCUS retrofits; updates input data
</commit_message>
<xml_diff>
--- a/InputData/elec/BBNPPTY/BAU Ban New Power Plants This Year.xlsx
+++ b/InputData/elec/BBNPPTY/BAU Ban New Power Plants This Year.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\elec\BBNPPTY\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Models\US\Models\eps-us\InputData\elec\BBNPPTY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7697ECBD-92C9-4103-9555-181ACE6C7B7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC7CBECA-90CF-4BE3-9075-5F308FED293B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="885" yWindow="1455" windowWidth="27360" windowHeight="21360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Source:</t>
   </si>
@@ -135,6 +135,12 @@
   </si>
   <si>
     <t>In the U.S., we use this to represent EPA 111 Rules. New coal without CCS is banned starting in</t>
+  </si>
+  <si>
+    <t>We also assume no new coal with CCS can be built prior to 2028 given the state of the technology</t>
+  </si>
+  <si>
+    <t>and the construction time for new or modified plants.</t>
   </si>
 </sst>
 </file>
@@ -517,10 +523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,6 +585,16 @@
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2028</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -594,8 +610,8 @@
   </sheetPr>
   <dimension ref="A1:AE25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E19" sqref="E19:H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2328,16 +2344,16 @@
         <v>1</v>
       </c>
       <c r="E19" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F19" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G19" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H19" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I19" s="5">
         <v>0</v>
@@ -2423,16 +2439,16 @@
         <v>1</v>
       </c>
       <c r="E20" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F20" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G20" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H20" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I20" s="5">
         <v>0</v>
@@ -2518,16 +2534,16 @@
         <v>1</v>
       </c>
       <c r="E21" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F21" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G21" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H21" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I21" s="5">
         <v>0</v>
@@ -2613,16 +2629,16 @@
         <v>1</v>
       </c>
       <c r="E22" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F22" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G22" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H22" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I22" s="5">
         <v>0</v>

</xml_diff>

<commit_message>
Historical year electricity calibration
</commit_message>
<xml_diff>
--- a/InputData/elec/BBNPPTY/BAU Ban New Power Plants This Year.xlsx
+++ b/InputData/elec/BBNPPTY/BAU Ban New Power Plants This Year.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Models\US\Models\eps-us\InputData\elec\BBNPPTY\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\elec\BBNPPTY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC7CBECA-90CF-4BE3-9075-5F308FED293B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E327A7F1-3EF2-40B1-8B65-730CF1661ABA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="885" yWindow="1455" windowWidth="27360" windowHeight="21360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -525,7 +525,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
@@ -610,8 +610,8 @@
   </sheetPr>
   <dimension ref="A1:AE25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19:H22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -720,13 +720,13 @@
         <v>11</v>
       </c>
       <c r="B2" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2" s="5">
         <v>0</v>
@@ -815,13 +815,13 @@
         <v>18</v>
       </c>
       <c r="B3" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" s="5">
         <v>0</v>
@@ -910,13 +910,13 @@
         <v>19</v>
       </c>
       <c r="B4" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" s="5">
         <v>0</v>
@@ -1005,13 +1005,13 @@
         <v>5</v>
       </c>
       <c r="B5" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" s="5">
         <v>0</v>
@@ -1100,13 +1100,13 @@
         <v>1</v>
       </c>
       <c r="B6" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" s="5">
         <v>0</v>
@@ -1195,13 +1195,13 @@
         <v>12</v>
       </c>
       <c r="B7" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7" s="5">
         <v>0</v>
@@ -1290,13 +1290,13 @@
         <v>3</v>
       </c>
       <c r="B8" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8" s="5">
         <v>0</v>
@@ -1385,13 +1385,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9" s="5">
         <v>0</v>
@@ -1480,13 +1480,13 @@
         <v>2</v>
       </c>
       <c r="B10" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D10" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10" s="5">
         <v>0</v>
@@ -1575,13 +1575,13 @@
         <v>7</v>
       </c>
       <c r="B11" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11" s="5">
         <v>0</v>
@@ -1670,13 +1670,13 @@
         <v>8</v>
       </c>
       <c r="B12" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D12" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E12" s="5">
         <v>0</v>
@@ -1765,13 +1765,13 @@
         <v>9</v>
       </c>
       <c r="B13" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D13" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E13" s="5">
         <v>0</v>
@@ -1860,13 +1860,13 @@
         <v>10</v>
       </c>
       <c r="B14" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D14" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E14" s="5">
         <v>0</v>
@@ -1955,13 +1955,13 @@
         <v>13</v>
       </c>
       <c r="B15" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C15" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D15" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E15" s="5">
         <v>0</v>
@@ -2050,13 +2050,13 @@
         <v>14</v>
       </c>
       <c r="B16" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C16" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D16" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E16" s="5">
         <v>0</v>
@@ -2145,13 +2145,13 @@
         <v>15</v>
       </c>
       <c r="B17" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D17" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E17" s="5">
         <v>0</v>
@@ -2240,13 +2240,13 @@
         <v>16</v>
       </c>
       <c r="B18" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C18" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D18" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E18" s="5">
         <v>0</v>
@@ -2715,13 +2715,13 @@
         <v>24</v>
       </c>
       <c r="B23" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C23" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D23" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E23" s="5">
         <v>0</v>
@@ -2810,13 +2810,13 @@
         <v>25</v>
       </c>
       <c r="B24" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C24" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D24" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E24" s="5">
         <v>0</v>
@@ -2905,13 +2905,13 @@
         <v>26</v>
       </c>
       <c r="B25" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C25" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D25" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E25" s="5">
         <v>0</v>

</xml_diff>

<commit_message>
Data updates to only use historical data (and prevent model builds) for historical years, and switch over to the model's capacity mechanisms for renewables specifically starting in 2024.
</commit_message>
<xml_diff>
--- a/InputData/elec/BBNPPTY/BAU Ban New Power Plants This Year.xlsx
+++ b/InputData/elec/BBNPPTY/BAU Ban New Power Plants This Year.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\elec\BBNPPTY\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Models\US\Models\eps-us\InputData\elec\BBNPPTY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E327A7F1-3EF2-40B1-8B65-730CF1661ABA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AED5C7C3-C6DD-4CC0-A75D-D5DA17DC76DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3900" yWindow="3900" windowWidth="38865" windowHeight="17235" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -611,7 +611,7 @@
   <dimension ref="A1:AE25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="B2" sqref="B2:D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -719,14 +719,14 @@
       <c r="A2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="5">
-        <v>0</v>
-      </c>
-      <c r="C2" s="5">
-        <v>0</v>
-      </c>
-      <c r="D2" s="5">
-        <v>0</v>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
       </c>
       <c r="E2" s="5">
         <v>0</v>
@@ -814,14 +814,14 @@
       <c r="A3" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="5">
-        <v>0</v>
-      </c>
-      <c r="C3" s="5">
-        <v>0</v>
-      </c>
-      <c r="D3" s="5">
-        <v>0</v>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
       </c>
       <c r="E3" s="5">
         <v>0</v>
@@ -909,14 +909,14 @@
       <c r="A4" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="5">
-        <v>0</v>
-      </c>
-      <c r="C4" s="5">
-        <v>0</v>
-      </c>
-      <c r="D4" s="5">
-        <v>0</v>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
       </c>
       <c r="E4" s="5">
         <v>0</v>
@@ -1004,14 +1004,14 @@
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="5">
-        <v>0</v>
-      </c>
-      <c r="C5" s="5">
-        <v>0</v>
-      </c>
-      <c r="D5" s="5">
-        <v>0</v>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
       </c>
       <c r="E5" s="5">
         <v>0</v>
@@ -1099,14 +1099,14 @@
       <c r="A6" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="5">
-        <v>0</v>
-      </c>
-      <c r="C6" s="5">
-        <v>0</v>
-      </c>
-      <c r="D6" s="5">
-        <v>0</v>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
       </c>
       <c r="E6" s="5">
         <v>0</v>
@@ -1194,14 +1194,14 @@
       <c r="A7" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="5">
-        <v>0</v>
-      </c>
-      <c r="C7" s="5">
-        <v>0</v>
-      </c>
-      <c r="D7" s="5">
-        <v>0</v>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
       </c>
       <c r="E7" s="5">
         <v>0</v>
@@ -1289,14 +1289,14 @@
       <c r="A8" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="5">
-        <v>0</v>
-      </c>
-      <c r="C8" s="5">
-        <v>0</v>
-      </c>
-      <c r="D8" s="5">
-        <v>0</v>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
       </c>
       <c r="E8" s="5">
         <v>0</v>
@@ -1384,14 +1384,14 @@
       <c r="A9" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="5">
-        <v>0</v>
-      </c>
-      <c r="C9" s="5">
-        <v>0</v>
-      </c>
-      <c r="D9" s="5">
-        <v>0</v>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
       </c>
       <c r="E9" s="5">
         <v>0</v>
@@ -1479,14 +1479,14 @@
       <c r="A10" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="5">
-        <v>0</v>
-      </c>
-      <c r="C10" s="5">
-        <v>0</v>
-      </c>
-      <c r="D10" s="5">
-        <v>0</v>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
       </c>
       <c r="E10" s="5">
         <v>0</v>
@@ -1574,14 +1574,14 @@
       <c r="A11" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="5">
-        <v>0</v>
-      </c>
-      <c r="C11" s="5">
-        <v>0</v>
-      </c>
-      <c r="D11" s="5">
-        <v>0</v>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
       </c>
       <c r="E11" s="5">
         <v>0</v>
@@ -1669,14 +1669,14 @@
       <c r="A12" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="5">
-        <v>0</v>
-      </c>
-      <c r="C12" s="5">
-        <v>0</v>
-      </c>
-      <c r="D12" s="5">
-        <v>0</v>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
       </c>
       <c r="E12" s="5">
         <v>0</v>
@@ -1764,14 +1764,14 @@
       <c r="A13" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="5">
-        <v>0</v>
-      </c>
-      <c r="C13" s="5">
-        <v>0</v>
-      </c>
-      <c r="D13" s="5">
-        <v>0</v>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
       </c>
       <c r="E13" s="5">
         <v>0</v>
@@ -1859,14 +1859,14 @@
       <c r="A14" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="5">
-        <v>0</v>
-      </c>
-      <c r="C14" s="5">
-        <v>0</v>
-      </c>
-      <c r="D14" s="5">
-        <v>0</v>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
       </c>
       <c r="E14" s="5">
         <v>0</v>
@@ -1954,14 +1954,14 @@
       <c r="A15" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="5">
-        <v>0</v>
-      </c>
-      <c r="C15" s="5">
-        <v>0</v>
-      </c>
-      <c r="D15" s="5">
-        <v>0</v>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
       </c>
       <c r="E15" s="5">
         <v>0</v>
@@ -2049,14 +2049,14 @@
       <c r="A16" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="5">
-        <v>0</v>
-      </c>
-      <c r="C16" s="5">
-        <v>0</v>
-      </c>
-      <c r="D16" s="5">
-        <v>0</v>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
       </c>
       <c r="E16" s="5">
         <v>0</v>
@@ -2144,14 +2144,14 @@
       <c r="A17" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="5">
-        <v>0</v>
-      </c>
-      <c r="C17" s="5">
-        <v>0</v>
-      </c>
-      <c r="D17" s="5">
-        <v>0</v>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
       </c>
       <c r="E17" s="5">
         <v>0</v>
@@ -2239,14 +2239,14 @@
       <c r="A18" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="5">
-        <v>0</v>
-      </c>
-      <c r="C18" s="5">
-        <v>0</v>
-      </c>
-      <c r="D18" s="5">
-        <v>0</v>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
       </c>
       <c r="E18" s="5">
         <v>0</v>
@@ -2334,13 +2334,13 @@
       <c r="A19" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="5">
-        <v>1</v>
-      </c>
-      <c r="C19" s="5">
-        <v>1</v>
-      </c>
-      <c r="D19" s="5">
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
         <v>1</v>
       </c>
       <c r="E19" s="5">
@@ -2429,13 +2429,13 @@
       <c r="A20" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="5">
-        <v>1</v>
-      </c>
-      <c r="C20" s="5">
-        <v>1</v>
-      </c>
-      <c r="D20" s="5">
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
         <v>1</v>
       </c>
       <c r="E20" s="5">
@@ -2524,13 +2524,13 @@
       <c r="A21" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="5">
-        <v>1</v>
-      </c>
-      <c r="C21" s="5">
-        <v>1</v>
-      </c>
-      <c r="D21" s="5">
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
         <v>1</v>
       </c>
       <c r="E21" s="5">
@@ -2619,13 +2619,13 @@
       <c r="A22" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="5">
-        <v>1</v>
-      </c>
-      <c r="C22" s="5">
-        <v>1</v>
-      </c>
-      <c r="D22" s="5">
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
         <v>1</v>
       </c>
       <c r="E22" s="5">
@@ -2714,14 +2714,14 @@
       <c r="A23" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="5">
-        <v>0</v>
-      </c>
-      <c r="C23" s="5">
-        <v>0</v>
-      </c>
-      <c r="D23" s="5">
-        <v>0</v>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
       </c>
       <c r="E23" s="5">
         <v>0</v>
@@ -2809,14 +2809,14 @@
       <c r="A24" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B24" s="5">
-        <v>0</v>
-      </c>
-      <c r="C24" s="5">
-        <v>0</v>
-      </c>
-      <c r="D24" s="5">
-        <v>0</v>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
       </c>
       <c r="E24" s="5">
         <v>0</v>
@@ -2904,14 +2904,14 @@
       <c r="A25" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B25" s="5">
-        <v>0</v>
-      </c>
-      <c r="C25" s="5">
-        <v>0</v>
-      </c>
-      <c r="D25" s="5">
-        <v>0</v>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
       </c>
       <c r="E25" s="5">
         <v>0</v>

</xml_diff>

<commit_message>
Block all offshore wind not currently planned/under construction in Current Policies
</commit_message>
<xml_diff>
--- a/InputData/elec/BBNPPTY/BAU Ban New Power Plants This Year.xlsx
+++ b/InputData/elec/BBNPPTY/BAU Ban New Power Plants This Year.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Models\US\Models\eps-us\InputData\elec\BBNPPTY\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\elec\BBNPPTY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AED5C7C3-C6DD-4CC0-A75D-D5DA17DC76DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E4ECCE7-AE75-4F86-9A13-97DB1F7FD9B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="3900" windowWidth="38865" windowHeight="17235" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>Source:</t>
   </si>
@@ -141,6 +141,15 @@
   </si>
   <si>
     <t>and the construction time for new or modified plants.</t>
+  </si>
+  <si>
+    <t>Due to recent blocks on offshore wind permitting and leasing, we assume only</t>
+  </si>
+  <si>
+    <t>already planned capacity (captured in elec/BPMCCS) will be built, and other</t>
+  </si>
+  <si>
+    <t>economic or reliability additions will not occur (offshore wind set to 1 in this file).</t>
   </si>
 </sst>
 </file>
@@ -523,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,6 +604,21 @@
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -610,8 +634,8 @@
   </sheetPr>
   <dimension ref="A1:AE25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D25"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15:AE15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1963,86 +1987,86 @@
       <c r="D15">
         <v>1</v>
       </c>
-      <c r="E15" s="5">
-        <v>0</v>
-      </c>
-      <c r="F15" s="5">
-        <v>0</v>
-      </c>
-      <c r="G15" s="5">
-        <v>0</v>
-      </c>
-      <c r="H15" s="5">
-        <v>0</v>
-      </c>
-      <c r="I15" s="5">
-        <v>0</v>
-      </c>
-      <c r="J15" s="5">
-        <v>0</v>
-      </c>
-      <c r="K15" s="5">
-        <v>0</v>
-      </c>
-      <c r="L15" s="5">
-        <v>0</v>
-      </c>
-      <c r="M15" s="5">
-        <v>0</v>
-      </c>
-      <c r="N15" s="5">
-        <v>0</v>
-      </c>
-      <c r="O15" s="5">
-        <v>0</v>
-      </c>
-      <c r="P15" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="5">
-        <v>0</v>
-      </c>
-      <c r="R15" s="5">
-        <v>0</v>
-      </c>
-      <c r="S15" s="5">
-        <v>0</v>
-      </c>
-      <c r="T15" s="5">
-        <v>0</v>
-      </c>
-      <c r="U15" s="5">
-        <v>0</v>
-      </c>
-      <c r="V15" s="5">
-        <v>0</v>
-      </c>
-      <c r="W15" s="5">
-        <v>0</v>
-      </c>
-      <c r="X15" s="5">
-        <v>0</v>
-      </c>
-      <c r="Y15" s="5">
-        <v>0</v>
-      </c>
-      <c r="Z15" s="5">
-        <v>0</v>
-      </c>
-      <c r="AA15" s="5">
-        <v>0</v>
-      </c>
-      <c r="AB15" s="5">
-        <v>0</v>
-      </c>
-      <c r="AC15" s="5">
-        <v>0</v>
-      </c>
-      <c r="AD15" s="5">
-        <v>0</v>
-      </c>
-      <c r="AE15" s="5">
-        <v>0</v>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <v>1</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="L15">
+        <v>1</v>
+      </c>
+      <c r="M15">
+        <v>1</v>
+      </c>
+      <c r="N15">
+        <v>1</v>
+      </c>
+      <c r="O15">
+        <v>1</v>
+      </c>
+      <c r="P15">
+        <v>1</v>
+      </c>
+      <c r="Q15">
+        <v>1</v>
+      </c>
+      <c r="R15">
+        <v>1</v>
+      </c>
+      <c r="S15">
+        <v>1</v>
+      </c>
+      <c r="T15">
+        <v>1</v>
+      </c>
+      <c r="U15">
+        <v>1</v>
+      </c>
+      <c r="V15">
+        <v>1</v>
+      </c>
+      <c r="W15">
+        <v>1</v>
+      </c>
+      <c r="X15">
+        <v>1</v>
+      </c>
+      <c r="Y15">
+        <v>1</v>
+      </c>
+      <c r="Z15">
+        <v>1</v>
+      </c>
+      <c r="AA15">
+        <v>1</v>
+      </c>
+      <c r="AB15">
+        <v>1</v>
+      </c>
+      <c r="AC15">
+        <v>1</v>
+      </c>
+      <c r="AD15">
+        <v>1</v>
+      </c>
+      <c r="AE15">
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update historical capacity additions; for BPMCCS, increase wind and solar additions to cover all capacity currently under construction
</commit_message>
<xml_diff>
--- a/InputData/elec/BBNPPTY/BAU Ban New Power Plants This Year.xlsx
+++ b/InputData/elec/BBNPPTY/BAU Ban New Power Plants This Year.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\elec\BBNPPTY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E4ECCE7-AE75-4F86-9A13-97DB1F7FD9B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27CAEC3F-A5CC-4DB3-92FD-C25CD6D7BCD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24120" yWindow="6690" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Source:</t>
   </si>
@@ -150,6 +150,12 @@
   </si>
   <si>
     <t>economic or reliability additions will not occur (offshore wind set to 1 in this file).</t>
+  </si>
+  <si>
+    <t>For historical years (2021-2024), we directly read in capacity additions in other input</t>
+  </si>
+  <si>
+    <t>data files and therefore disallow additional economic additions.</t>
   </si>
 </sst>
 </file>
@@ -532,23 +538,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="60.85546875" customWidth="1"/>
+    <col min="2" max="2" width="60.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -556,69 +562,79 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B5" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B6" s="3">
         <v>2024</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B7" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>2028</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -634,17 +650,17 @@
   </sheetPr>
   <dimension ref="A1:AE25"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15:AE15"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" customWidth="1"/>
-    <col min="2" max="2" width="27.28515625" customWidth="1"/>
+    <col min="1" max="1" width="26.453125" customWidth="1"/>
+    <col min="2" max="2" width="27.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -739,7 +755,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -752,8 +768,8 @@
       <c r="D2">
         <v>1</v>
       </c>
-      <c r="E2" s="5">
-        <v>0</v>
+      <c r="E2">
+        <v>1</v>
       </c>
       <c r="F2" s="5">
         <v>0</v>
@@ -834,7 +850,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -847,8 +863,8 @@
       <c r="D3">
         <v>1</v>
       </c>
-      <c r="E3" s="5">
-        <v>0</v>
+      <c r="E3">
+        <v>1</v>
       </c>
       <c r="F3" s="5">
         <v>0</v>
@@ -929,7 +945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -942,8 +958,8 @@
       <c r="D4">
         <v>1</v>
       </c>
-      <c r="E4" s="5">
-        <v>0</v>
+      <c r="E4">
+        <v>1</v>
       </c>
       <c r="F4" s="5">
         <v>0</v>
@@ -1024,7 +1040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1037,8 +1053,8 @@
       <c r="D5">
         <v>1</v>
       </c>
-      <c r="E5" s="5">
-        <v>0</v>
+      <c r="E5">
+        <v>1</v>
       </c>
       <c r="F5" s="5">
         <v>0</v>
@@ -1119,7 +1135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -1132,8 +1148,8 @@
       <c r="D6">
         <v>1</v>
       </c>
-      <c r="E6" s="5">
-        <v>0</v>
+      <c r="E6">
+        <v>1</v>
       </c>
       <c r="F6" s="5">
         <v>0</v>
@@ -1214,7 +1230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1227,8 +1243,8 @@
       <c r="D7">
         <v>1</v>
       </c>
-      <c r="E7" s="5">
-        <v>0</v>
+      <c r="E7">
+        <v>1</v>
       </c>
       <c r="F7" s="5">
         <v>0</v>
@@ -1309,7 +1325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -1322,8 +1338,8 @@
       <c r="D8">
         <v>1</v>
       </c>
-      <c r="E8" s="5">
-        <v>0</v>
+      <c r="E8">
+        <v>1</v>
       </c>
       <c r="F8" s="5">
         <v>0</v>
@@ -1404,7 +1420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -1417,8 +1433,8 @@
       <c r="D9">
         <v>1</v>
       </c>
-      <c r="E9" s="5">
-        <v>0</v>
+      <c r="E9">
+        <v>1</v>
       </c>
       <c r="F9" s="5">
         <v>0</v>
@@ -1499,7 +1515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -1512,8 +1528,8 @@
       <c r="D10">
         <v>1</v>
       </c>
-      <c r="E10" s="5">
-        <v>0</v>
+      <c r="E10">
+        <v>1</v>
       </c>
       <c r="F10" s="5">
         <v>0</v>
@@ -1594,7 +1610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -1607,8 +1623,8 @@
       <c r="D11">
         <v>1</v>
       </c>
-      <c r="E11" s="5">
-        <v>0</v>
+      <c r="E11">
+        <v>1</v>
       </c>
       <c r="F11" s="5">
         <v>0</v>
@@ -1689,7 +1705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -1702,8 +1718,8 @@
       <c r="D12">
         <v>1</v>
       </c>
-      <c r="E12" s="5">
-        <v>0</v>
+      <c r="E12">
+        <v>1</v>
       </c>
       <c r="F12" s="5">
         <v>0</v>
@@ -1784,7 +1800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -1797,8 +1813,8 @@
       <c r="D13">
         <v>1</v>
       </c>
-      <c r="E13" s="5">
-        <v>0</v>
+      <c r="E13">
+        <v>1</v>
       </c>
       <c r="F13" s="5">
         <v>0</v>
@@ -1879,7 +1895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -1892,8 +1908,8 @@
       <c r="D14">
         <v>1</v>
       </c>
-      <c r="E14" s="5">
-        <v>0</v>
+      <c r="E14">
+        <v>1</v>
       </c>
       <c r="F14" s="5">
         <v>0</v>
@@ -1974,7 +1990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -2069,7 +2085,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -2082,8 +2098,8 @@
       <c r="D16">
         <v>1</v>
       </c>
-      <c r="E16" s="5">
-        <v>0</v>
+      <c r="E16">
+        <v>1</v>
       </c>
       <c r="F16" s="5">
         <v>0</v>
@@ -2164,7 +2180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -2177,8 +2193,8 @@
       <c r="D17">
         <v>1</v>
       </c>
-      <c r="E17" s="5">
-        <v>0</v>
+      <c r="E17">
+        <v>1</v>
       </c>
       <c r="F17" s="5">
         <v>0</v>
@@ -2259,7 +2275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -2272,8 +2288,8 @@
       <c r="D18">
         <v>1</v>
       </c>
-      <c r="E18" s="5">
-        <v>0</v>
+      <c r="E18">
+        <v>1</v>
       </c>
       <c r="F18" s="5">
         <v>0</v>
@@ -2354,7 +2370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -2367,7 +2383,7 @@
       <c r="D19">
         <v>1</v>
       </c>
-      <c r="E19" s="5">
+      <c r="E19">
         <v>1</v>
       </c>
       <c r="F19" s="5">
@@ -2449,7 +2465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -2462,7 +2478,7 @@
       <c r="D20">
         <v>1</v>
       </c>
-      <c r="E20" s="5">
+      <c r="E20">
         <v>1</v>
       </c>
       <c r="F20" s="5">
@@ -2544,7 +2560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -2557,7 +2573,7 @@
       <c r="D21">
         <v>1</v>
       </c>
-      <c r="E21" s="5">
+      <c r="E21">
         <v>1</v>
       </c>
       <c r="F21" s="5">
@@ -2639,7 +2655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -2652,7 +2668,7 @@
       <c r="D22">
         <v>1</v>
       </c>
-      <c r="E22" s="5">
+      <c r="E22">
         <v>1</v>
       </c>
       <c r="F22" s="5">
@@ -2734,7 +2750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -2747,8 +2763,8 @@
       <c r="D23">
         <v>1</v>
       </c>
-      <c r="E23" s="5">
-        <v>0</v>
+      <c r="E23">
+        <v>1</v>
       </c>
       <c r="F23" s="5">
         <v>0</v>
@@ -2829,7 +2845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A24" s="6" t="s">
         <v>25</v>
       </c>
@@ -2842,8 +2858,8 @@
       <c r="D24">
         <v>1</v>
       </c>
-      <c r="E24" s="5">
-        <v>0</v>
+      <c r="E24">
+        <v>1</v>
       </c>
       <c r="F24" s="5">
         <v>0</v>
@@ -2924,7 +2940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A25" s="6" t="s">
         <v>26</v>
       </c>
@@ -2937,8 +2953,8 @@
       <c r="D25">
         <v>1</v>
       </c>
-      <c r="E25" s="5">
-        <v>0</v>
+      <c r="E25">
+        <v>1</v>
       </c>
       <c r="F25" s="5">
         <v>0</v>

</xml_diff>